<commit_message>
PDF export functionality added + some refactoring.
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -783,15 +783,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
@@ -818,15 +818,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
@@ -853,15 +853,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
@@ -888,15 +888,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
@@ -1083,7 +1083,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -1144,7 +1144,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="0">
-        <v>3.67</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -1152,7 +1152,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="1">
-        <v>3.89</v>
+        <v>3.94</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +1230,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0">
-        <v>3.67</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -1238,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1">
-        <v>3.89</v>
+        <v>3.94</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>